<commit_message>
Added three AH sensors power, E-today and E-total
</commit_message>
<xml_diff>
--- a/debug_payload/message.xlsx
+++ b/debug_payload/message.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73b08471db47a260/Archive/Erik/Hobby/Domotica/Omnik2MQTT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73b08471db47a260/Documents/GitHub/omnik2mqttproxy/debug_payload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="11_F25DC773A252ABDACC10487E895D68EE5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80EFFE63-8189-4586-A643-985A43FBAD6A}"/>
+  <xr:revisionPtr revIDLastSave="623" documentId="11_F25DC773A252ABDACC10487E895D68EE5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6538265-6FA1-4C82-9F41-036819B43A8D}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-11496" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
   <si>
     <t>68:7D:41:B0:5D:1F:19:24:5D:1F:19:24:81:02:01:4E:4C:44:4E:31:35:32:30:31:33:38:43:31:30:30:31:01:9D:07:7F:00:00:FF:FF:00:0F:00:B4:FF:FF:00:0B:FF:FF:FF:FF:09:20:FF:FF:FF:FF:13:8F:01:10:FF:FF:FF:FF:FF:FF:FF:FF:00:9B:00:01:7B:01:00:00:9A:97:00:01:00:00:00:00:FF:FF:00:00:00:00:00:00:00:00:00:00:4E:4C:31:2D:56:31:2E:30:2D:30:30:34:33:2D:34:00:00:00:00:00:56:31:2E:36:2D:30:30:31:38:00:00:00:00:00:00:00:00:00:00:00:0E:16:</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>2x (5d 1f 19 24)</t>
+  </si>
+  <si>
+    <t>UDP Message 2</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,12 +506,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -884,6 +881,9 @@
       <c r="K11" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="M11" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
@@ -896,20 +896,20 @@
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="3" t="s">
         <v>124</v>
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="8">
+      <c r="I12" s="2">
         <v>68</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
         <v>68</v>
       </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2">
         <v>68</v>
       </c>
     </row>
@@ -922,17 +922,17 @@
         <f>B13+D13</f>
         <v>4</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="2" t="s">
         <v>125</v>
       </c>
       <c r="J13" s="5"/>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="2" t="s">
         <v>125</v>
       </c>
       <c r="M13" t="s">

</xml_diff>

<commit_message>
Major upgrade in posting mqtt updates
</commit_message>
<xml_diff>
--- a/debug_payload/message.xlsx
+++ b/debug_payload/message.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73b08471db47a260/Documents/GitHub/omnik2mqttproxy/debug_payload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="623" documentId="11_F25DC773A252ABDACC10487E895D68EE5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6538265-6FA1-4C82-9F41-036819B43A8D}"/>
+  <xr:revisionPtr revIDLastSave="774" documentId="11_F25DC773A252ABDACC10487E895D68EE5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB425D02-0DAD-4276-80D5-AA5255507A55}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-11496" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-11496" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="179">
   <si>
     <t>68:7D:41:B0:5D:1F:19:24:5D:1F:19:24:81:02:01:4E:4C:44:4E:31:35:32:30:31:33:38:43:31:30:30:31:01:9D:07:7F:00:00:FF:FF:00:0F:00:B4:FF:FF:00:0B:FF:FF:FF:FF:09:20:FF:FF:FF:FF:13:8F:01:10:FF:FF:FF:FF:FF:FF:FF:FF:00:9B:00:01:7B:01:00:00:9A:97:00:01:00:00:00:00:FF:FF:00:00:00:00:00:00:00:00:00:00:4E:4C:31:2D:56:31:2E:30:2D:30:30:34:33:2D:34:00:00:00:00:00:56:31:2E:36:2D:30:30:31:38:00:00:00:00:00:00:00:00:00:00:00:0E:16:</t>
   </si>
@@ -284,9 +286,6 @@
     <t xml:space="preserve"> 09 30 ff ff ff ff </t>
   </si>
   <si>
-    <t>/11</t>
-  </si>
-  <si>
     <t>/12</t>
   </si>
   <si>
@@ -377,9 +376,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Total invertor</t>
-  </si>
-  <si>
     <t>Verschil</t>
   </si>
   <si>
@@ -441,13 +437,151 @@
   </si>
   <si>
     <t>UDP Message 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solarmanpv</t>
+  </si>
+  <si>
+    <t>inverter</t>
+  </si>
+  <si>
+    <t>0x0118</t>
+  </si>
+  <si>
+    <t>0x00AC</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>"aH1BsF0fGSRdHxkkgQIBTkxETjE1MjAxMzhDMTAwMQFiBv0AAP//AAcAs///AAT/////CTD/////E4wAbP//////////AK0AAXsqAACavAABAAAAAP//AAAAAAAAAAAAAE5MMS1WMS4wLTAwNDMtNAAAAAAAVjEuNi0wMDE4AAAAAAAAAAAAAAAIFg==\n"</t>
+  </si>
+  <si>
+    <t>Current power</t>
+  </si>
+  <si>
+    <t>Today energy</t>
+  </si>
+  <si>
+    <t>1,73</t>
+  </si>
+  <si>
+    <t>Total energy</t>
+  </si>
+  <si>
+    <t>9.706,6</t>
+  </si>
+  <si>
+    <t>Inverter temperature</t>
+  </si>
+  <si>
+    <t>35,4</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>1.679.416.367,56</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>21 maart 2023 om 17:32:47</t>
+  </si>
+  <si>
+    <t>687D41B05D1F19245D1F19248102014E4C444E313532303133384331303031016206FD0000FFFF000700B3FFFF0004FFFFFFFF0930FFFFFFFF138C006CFFFFFFFFFFFFFFFF00AD00017B2A00009ABC000100000000FFFF000000000000000000004E4C312D56312E302D303034332D34000000000056312E362D3030313800000000000000000000000816</t>
+  </si>
+  <si>
+    <t>7D41B0</t>
+  </si>
+  <si>
+    <t>5D1F19245D1F1924</t>
+  </si>
+  <si>
+    <t>4E4C444E313532303133384331303031</t>
+  </si>
+  <si>
+    <t>0162</t>
+  </si>
+  <si>
+    <t>06FD</t>
+  </si>
+  <si>
+    <t>0000FFFF</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>00B3</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>FFFFFFFF</t>
+  </si>
+  <si>
+    <t>0930</t>
+  </si>
+  <si>
+    <t>138C</t>
+  </si>
+  <si>
+    <t>006C</t>
+  </si>
+  <si>
+    <t>FFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>00AD</t>
+  </si>
+  <si>
+    <t>00017B2A</t>
+  </si>
+  <si>
+    <t>00009ABC</t>
+  </si>
+  <si>
+    <t>000100000000FFFF00000000000000000000</t>
+  </si>
+  <si>
+    <t>4E4C312D56312E302D303034332D34</t>
+  </si>
+  <si>
+    <t>0000000000</t>
+  </si>
+  <si>
+    <t>56312E362D30303138</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Hrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +602,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF212121"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -490,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -506,6 +645,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,6 +954,7 @@
     <col min="11" max="11" width="41.81640625" customWidth="1"/>
     <col min="12" max="12" width="16.08984375" customWidth="1"/>
     <col min="13" max="13" width="54" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.35">
@@ -843,18 +996,18 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.35">
@@ -882,7 +1035,7 @@
         <v>43</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
@@ -897,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" s="4"/>
       <c r="H12" s="4"/>
@@ -929,14 +1082,14 @@
       <c r="F13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" t="s">
         <v>125</v>
-      </c>
-      <c r="M13" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.35">
@@ -952,19 +1105,19 @@
         <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" t="s">
         <v>128</v>
       </c>
-      <c r="K14" t="s">
-        <v>130</v>
-      </c>
       <c r="M14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O14">
         <v>2013</v>
@@ -987,10 +1140,10 @@
       </c>
       <c r="E15" s="3"/>
       <c r="I15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" t="s">
         <v>129</v>
-      </c>
-      <c r="K15" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.35">
@@ -1006,7 +1159,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1018,10 +1171,10 @@
         <v>46</v>
       </c>
       <c r="L16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O16">
         <f>O14+1</f>
@@ -1063,10 +1216,10 @@
         <v>47</v>
       </c>
       <c r="L17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O25" si="3">O16+1</f>
@@ -1092,7 +1245,7 @@
         <v>66</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
         <v>68</v>
@@ -1104,10 +1257,10 @@
         <v>77</v>
       </c>
       <c r="L18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
@@ -1133,7 +1286,7 @@
         <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
         <v>68</v>
@@ -1145,7 +1298,7 @@
         <v>78</v>
       </c>
       <c r="L19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M19" s="2">
         <v>16</v>
@@ -1174,7 +1327,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>68</v>
@@ -1206,7 +1359,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
         <v>69</v>
@@ -1241,7 +1394,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="G22" t="s">
         <v>69</v>
@@ -1273,7 +1426,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
@@ -1305,7 +1458,7 @@
         <v>55</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s">
         <v>71</v>
@@ -1340,7 +1493,7 @@
         <v>53</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s">
         <v>71</v>
@@ -1372,7 +1525,7 @@
         <v>54</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
         <v>71</v>
@@ -1401,7 +1554,7 @@
         <v>56</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="G27" t="s">
         <v>70</v>
@@ -1433,7 +1586,7 @@
         <v>58</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="G28" t="s">
         <v>70</v>
@@ -1442,13 +1595,13 @@
         <v>14</v>
       </c>
       <c r="O28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P28">
         <v>17.440000000000001</v>
       </c>
       <c r="Q28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.35">
@@ -1467,7 +1620,7 @@
         <v>57</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="G29" t="s">
         <v>70</v>
@@ -1475,14 +1628,14 @@
       <c r="I29" t="s">
         <v>50</v>
       </c>
-      <c r="O29" t="s">
-        <v>112</v>
+      <c r="O29" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="P29">
         <v>17440</v>
       </c>
       <c r="Q29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.35">
@@ -1513,17 +1666,17 @@
         <v>5006</v>
       </c>
       <c r="K30" t="s">
-        <v>94</v>
-      </c>
-      <c r="O30" t="s">
-        <v>113</v>
+        <v>93</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="P30">
         <f>J37/10</f>
         <v>9703.6</v>
       </c>
       <c r="Q30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.35">
@@ -1542,7 +1695,7 @@
         <v>60</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
         <v>73</v>
@@ -1554,10 +1707,10 @@
         <v>107</v>
       </c>
       <c r="K31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P31">
         <f>P29-P30</f>
@@ -1589,10 +1742,10 @@
         <v>50</v>
       </c>
       <c r="K32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33" s="3">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -1614,7 +1767,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34" s="3">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -1639,7 +1792,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="3">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -1660,8 +1813,11 @@
       <c r="I35" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="L35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36" s="3">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1690,10 +1846,13 @@
         <v>52</v>
       </c>
       <c r="K36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="L36">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B37" s="3">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1722,13 +1881,13 @@
         <v>97036</v>
       </c>
       <c r="K37" t="s">
-        <v>99</v>
-      </c>
-      <c r="M37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="L37">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B38" s="3">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1752,10 +1911,13 @@
         <v>44</v>
       </c>
       <c r="K38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="L38" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B39" s="3">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1777,7 +1939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40" s="3">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -1794,10 +1956,10 @@
         <v>21</v>
       </c>
       <c r="K40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41" s="3">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1814,10 +1976,10 @@
         <v>22</v>
       </c>
       <c r="K41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42" s="3">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -1837,10 +1999,10 @@
         <v>23</v>
       </c>
       <c r="K42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B43" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1857,10 +2019,10 @@
         <v>26</v>
       </c>
       <c r="K43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B44" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1880,10 +2042,10 @@
         <v>27</v>
       </c>
       <c r="K44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B45" s="3">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -1903,7 +2065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46" s="3">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -1917,17 +2079,17 @@
       </c>
       <c r="E46" s="3"/>
       <c r="G46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I46" t="s">
         <v>29</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47" s="3">
         <f t="shared" si="1"/>
         <v>138</v>
@@ -1940,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I47" s="2">
         <v>16</v>
@@ -1949,6 +2111,1158 @@
       <c r="K47" s="2">
         <v>16</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A4696E-C08C-4F5B-B831-355C41C9D771}">
+  <dimension ref="A2:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="68.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="28.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="19" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="19" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="28.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B21396-4FF7-49AC-8DFA-02BD9A0BA8A6}">
+  <dimension ref="B3:R47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.26953125" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" customWidth="1"/>
+    <col min="11" max="11" width="5.90625" customWidth="1"/>
+    <col min="12" max="12" width="15.08984375" customWidth="1"/>
+    <col min="13" max="13" width="16.08984375" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <f>B12+D12</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12">
+        <v>68</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <f>C12</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <f>B13+D13</f>
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B14" s="3">
+        <f>C13</f>
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <f>B14+D14</f>
+        <v>12</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" t="s">
+        <v>152</v>
+      </c>
+      <c r="P14">
+        <v>2013</v>
+      </c>
+      <c r="Q14">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:B47" si="0">C14</f>
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <f>B15+D15</f>
+        <v>15</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="I15">
+        <v>810201</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <f>B16+D16</f>
+        <v>31</v>
+      </c>
+      <c r="D16" s="3">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>153</v>
+      </c>
+      <c r="P16">
+        <f>P14+1</f>
+        <v>2014</v>
+      </c>
+      <c r="Q16">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ref="C17:C47" si="1">B17+D17</f>
+        <v>33</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J17">
+        <v>35.4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>177</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P25" si="2">P16+1</f>
+        <v>2015</v>
+      </c>
+      <c r="Q17">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" t="s">
+        <v>155</v>
+      </c>
+      <c r="J18">
+        <v>178.9</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="Q18">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="P19">
+        <f t="shared" si="2"/>
+        <v>2017</v>
+      </c>
+      <c r="Q19">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>2018</v>
+      </c>
+      <c r="Q20">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J21">
+        <v>0.7</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>2019</v>
+      </c>
+      <c r="Q21">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>2020</v>
+      </c>
+      <c r="Q22">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>2021</v>
+      </c>
+      <c r="Q23">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B24" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J24">
+        <v>0.4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>176</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>2022</v>
+      </c>
+      <c r="Q24">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B25" s="3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>161</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="Q25">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B26" s="3">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q26" s="6">
+        <f>SUM(Q14:Q25)</f>
+        <v>17.391999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B27" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J27">
+        <v>235.2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B28" s="3">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P28" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q28">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="R28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B29" s="3">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q29">
+        <v>17440</v>
+      </c>
+      <c r="R29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" t="s">
+        <v>163</v>
+      </c>
+      <c r="J30">
+        <v>50.04</v>
+      </c>
+      <c r="K30" t="s">
+        <v>174</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q30">
+        <f>J37</f>
+        <v>9706.6</v>
+      </c>
+      <c r="R30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J31">
+        <v>108</v>
+      </c>
+      <c r="K31" t="s">
+        <v>173</v>
+      </c>
+      <c r="P31" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q31">
+        <f>Q29-Q30</f>
+        <v>7733.4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B35" s="3">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="D35" s="3">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B36" s="3">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36">
+        <v>1.73</v>
+      </c>
+      <c r="K36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M36">
+        <v>2.8</v>
+      </c>
+      <c r="N36" t="s">
+        <v>109</v>
+      </c>
+      <c r="O36">
+        <f>M36/J36</f>
+        <v>1.6184971098265895</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B37" s="3">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J37">
+        <v>9706.6</v>
+      </c>
+      <c r="K37" t="s">
+        <v>109</v>
+      </c>
+      <c r="M37">
+        <v>17440</v>
+      </c>
+      <c r="N37" t="s">
+        <v>109</v>
+      </c>
+      <c r="O37">
+        <f>M37/J37</f>
+        <v>1.7967156367832195</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B38" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38">
+        <v>39612</v>
+      </c>
+      <c r="K38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B39" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="J39">
+        <v>1500</v>
+      </c>
+      <c r="M39">
+        <v>2000</v>
+      </c>
+      <c r="O39">
+        <f>M39/J39</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B40" s="3">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="D40" s="3">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B41" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="D41" s="3">
+        <v>12</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="I41" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B42" s="3">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="D42" s="3">
+        <v>15</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B43" s="3">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="D43" s="3">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="I43" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B44" s="3">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="D44" s="3">
+        <v>9</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="G44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B45" s="3">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="D45" s="3">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B46" s="3">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="G46" t="s">
+        <v>106</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B47" s="3">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>107</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>